<commit_message>
All STM32 pins assigned. Applying changes on schematic.
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
+++ b/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="205">
   <si>
     <t>Pin #</t>
   </si>
@@ -214,12 +214,6 @@
   </si>
   <si>
     <t>OSC_OUT</t>
-  </si>
-  <si>
-    <t>Required for the USB function</t>
-  </si>
-  <si>
-    <t>PC13 has restrictions - check if connected properly</t>
   </si>
   <si>
     <r>
@@ -909,9 +903,6 @@
     <t>USART1_RX(8)</t>
   </si>
   <si>
-    <t>Can be used on PowerBoard if we have enough GPIOs already | If connected to SmartFusion it would be nice to have the UART functionality</t>
-  </si>
-  <si>
     <t>USBDM</t>
   </si>
   <si>
@@ -1031,24 +1022,15 @@
     <t>JTDI</t>
   </si>
   <si>
-    <t>TIM2_CH1_ETR/PA15/SPI1_NSS</t>
-  </si>
-  <si>
     <t>JTDO</t>
   </si>
   <si>
     <t>JNTRST</t>
   </si>
   <si>
-    <t>TIM3_CH1/PB4/SPI1_MISO</t>
-  </si>
-  <si>
     <t>I2C1_SMBA</t>
   </si>
   <si>
-    <t>TIM3_CH2/SPI1_MOSI</t>
-  </si>
-  <si>
     <t>USART1_RX</t>
   </si>
   <si>
@@ -1081,53 +1063,6 @@
   </si>
   <si>
     <t>I2C1_SDA</t>
-  </si>
-  <si>
-    <r>
-      <t>I</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> signals</t>
-    </r>
   </si>
   <si>
     <t>Boot mode selector pin</t>
@@ -1204,18 +1139,6 @@
     <t>LED1</t>
   </si>
   <si>
-    <t>External ?? MHz crystal</t>
-  </si>
-  <si>
-    <t>Double check clock synthesis options (USB, ADC, "natural" timer, UART)</t>
-  </si>
-  <si>
-    <t>GND pin connections (DGND?, pin visibility) connect to DGND (also on schematic)</t>
-  </si>
-  <si>
-    <t>Connect to GND via resistor</t>
-  </si>
-  <si>
     <t xml:space="preserve">NOTES: </t>
   </si>
   <si>
@@ -1225,12 +1148,6 @@
     <t>Connect !AL signal from battery gauge to a timer capture pin</t>
   </si>
   <si>
-    <t>JNTRST/PB4 | Check if this needed for SWD-based programming/debugging</t>
-  </si>
-  <si>
-    <t>May be used on PowerBoard instead | Priority to ILIM</t>
-  </si>
-  <si>
     <t>Master external power switch with pull up/down (initial condition)</t>
   </si>
   <si>
@@ -1249,9 +1166,6 @@
     <t>LED1 (GREEN)</t>
   </si>
   <si>
-    <t>LED2 (ORANGE) / BOOT1</t>
-  </si>
-  <si>
     <t>LED2</t>
   </si>
   <si>
@@ -1261,9 +1175,6 @@
     <t>GPIO x2 | OSC32</t>
   </si>
   <si>
-    <t>GPIO x3 | UART1</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1314,15 +1225,45 @@
     <t>SWCLK</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TIM2_CH2/PB3</t>
-    </r>
+    <t>TRACESWO</t>
+  </si>
+  <si>
+    <t>Weak pull-up for BOOT1 = '1' on startup</t>
+  </si>
+  <si>
+    <t>GPIO+</t>
+  </si>
+  <si>
+    <t>ILIM0</t>
+  </si>
+  <si>
+    <t>ILIM1</t>
+  </si>
+  <si>
+    <t>EN3 (?)</t>
+  </si>
+  <si>
+    <t>PWR_ON (?)</t>
+  </si>
+  <si>
+    <t>#AL/CC+</t>
+  </si>
+  <si>
+    <t>Header type: SAMTEC FSTH (2x5 50mil)</t>
+  </si>
+  <si>
+    <t>External 16 MHz crystal</t>
+  </si>
+  <si>
+    <t>Main clock source</t>
+  </si>
+  <si>
+    <t>USB clock requirements restrict SYSCLK to be 48 MHz or 72 MHz</t>
+  </si>
+  <si>
+    <t>LED2 (ORANGE) &amp; BOOT1</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1331,6 +1272,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>TIM3_CH2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/SPI1_MOSI</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TIM3_CH1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>/</t>
     </r>
     <r>
@@ -1342,6 +1315,71 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t>PB4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/SPI1_MISO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TIM2_CH1_ETR/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFA7D00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PA15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/SPI1_NSS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TIM2_CH2/PB3/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFA7D00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>TRACESWO</t>
     </r>
     <r>
@@ -1355,52 +1393,137 @@
     </r>
   </si>
   <si>
-    <t>TRACESWO</t>
-  </si>
-  <si>
-    <t>Weak pull-up for BOOT1 = '1' on startup</t>
-  </si>
-  <si>
-    <t>GPIO+</t>
-  </si>
-  <si>
-    <t>GPIO+ x2 (ILIM0, ILIM1)</t>
-  </si>
-  <si>
-    <t>GPIO+ x2 (EN3)</t>
-  </si>
-  <si>
-    <t>ILIM0</t>
-  </si>
-  <si>
-    <t>ILIM1</t>
-  </si>
-  <si>
-    <t>EN3 (?)</t>
-  </si>
-  <si>
-    <t>PWR_ON (?)</t>
-  </si>
-  <si>
-    <t>#EXTPWR (?)</t>
-  </si>
-  <si>
-    <t>#AL/CC+</t>
-  </si>
-  <si>
-    <t>Check if I2C configurable</t>
-  </si>
-  <si>
-    <t>Check if I2C readable</t>
-  </si>
-  <si>
-    <t>Header type: SAMTEC FSTH (2x5 50mil)</t>
-  </si>
-  <si>
-    <t>Check TIM2_CH1_ETR meaning</t>
-  </si>
-  <si>
-    <t>Check if I2C can be used for turning off/on BUCK3</t>
+    <t>MASTER SWITCH</t>
+  </si>
+  <si>
+    <t>LTC2942-1</t>
+  </si>
+  <si>
+    <t>3-pin JUMPER</t>
+  </si>
+  <si>
+    <t>Set to 100 mA by default</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LIM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> selector</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> signals | USART</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> signals</t>
+    </r>
+  </si>
+  <si>
+    <t>Master switch</t>
+  </si>
+  <si>
+    <t>#EXTPWR</t>
+  </si>
+  <si>
+    <t>LTC3677</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>Always on</t>
+  </si>
+  <si>
+    <t>SWD signal</t>
+  </si>
+  <si>
+    <t>Power switch for ALL rails</t>
+  </si>
+  <si>
+    <t>EN3</t>
+  </si>
+  <si>
+    <t>Battery Gauge #AL/CC</t>
   </si>
 </sst>
 </file>
@@ -1500,15 +1623,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1543,11 +1666,11 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1595,15 +1718,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1613,12 +1727,18 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1628,9 +1748,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1650,9 +1770,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1677,16 +1794,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyAlignment="1">
@@ -1696,7 +1807,24 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1705,57 +1833,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1764,8 +1883,8 @@
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Good" xfId="4" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="5" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2057,10 +2176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44:J45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I44" sqref="I44:I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2069,62 +2188,62 @@
     <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="63.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="24" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="29" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="11" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="1:10" ht="30.75" thickBot="1">
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+    </row>
+    <row r="3" spans="1:10" ht="30">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -2143,18 +2262,18 @@
       <c r="F3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>174</v>
+      <c r="G3" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="21"/>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -2173,21 +2292,19 @@
       <c r="F4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="H4" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickTop="1">
-      <c r="A5" s="18">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -2199,27 +2316,27 @@
       <c r="D5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>60</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>176</v>
+      <c r="H5" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A6" s="18">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -2231,21 +2348,21 @@
       <c r="D6" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="18" t="s">
+      <c r="F6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="34"/>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A7" s="15">
+      <c r="H6" s="43"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="31"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -2260,24 +2377,24 @@
       <c r="E7" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="I7" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickTop="1">
-      <c r="A8" s="15">
+      <c r="H7" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="I7" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="J7" s="37" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="25">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -2289,20 +2406,18 @@
       <c r="D8" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="20" t="s">
-        <v>165</v>
-      </c>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="2">
@@ -2317,23 +2432,23 @@
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>177</v>
+      <c r="H9" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>181</v>
+        <v>138</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18">
@@ -2341,60 +2456,60 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>73</v>
+        <v>79</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>71</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="27"/>
+      <c r="J10" s="34"/>
     </row>
     <row r="11" spans="1:10" ht="18">
       <c r="A11" s="2">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>56</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="27"/>
+      <c r="J11" s="34"/>
     </row>
     <row r="12" spans="1:10" s="5" customFormat="1" ht="32.25" customHeight="1">
       <c r="A12" s="2">
@@ -2407,20 +2522,20 @@
         <v>47</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J12" s="2"/>
     </row>
@@ -2437,17 +2552,17 @@
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>75</v>
+      <c r="E13" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30">
@@ -2463,17 +2578,17 @@
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>76</v>
+      <c r="E14" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30">
@@ -2489,17 +2604,17 @@
       <c r="D15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>77</v>
+      <c r="E15" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30">
@@ -2515,22 +2630,22 @@
       <c r="D16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>83</v>
+      <c r="E16" s="8" t="s">
+        <v>81</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H16" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="I16" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="J16" s="27"/>
+        <v>85</v>
+      </c>
+      <c r="H16" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="J16" s="34"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="2">
@@ -2545,18 +2660,18 @@
       <c r="D17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>84</v>
+      <c r="E17" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="27"/>
+        <v>86</v>
+      </c>
+      <c r="H17" s="43"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="34"/>
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="A18" s="2">
@@ -2571,18 +2686,18 @@
       <c r="D18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>85</v>
+      <c r="E18" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="27"/>
+        <v>87</v>
+      </c>
+      <c r="H18" s="43"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="34"/>
     </row>
     <row r="19" spans="1:10" ht="30">
       <c r="A19" s="2">
@@ -2597,18 +2712,18 @@
       <c r="D19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="9" t="s">
-        <v>86</v>
+      <c r="E19" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="27"/>
+        <v>88</v>
+      </c>
+      <c r="H19" s="43"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="2">
@@ -2623,18 +2738,18 @@
       <c r="D20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2650,22 +2765,22 @@
       <c r="D21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="18">
+      <c r="A22" s="16">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2675,7 +2790,7 @@
         <v>47</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>56</v>
@@ -2683,17 +2798,17 @@
       <c r="F22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>190</v>
+      <c r="H22" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1">
@@ -2709,22 +2824,22 @@
       <c r="D23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="H23" s="31" t="s">
+      <c r="I23" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="I23" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="J23" s="27"/>
+      <c r="J23" s="34"/>
     </row>
     <row r="24" spans="1:10" ht="30">
       <c r="A24" s="2">
@@ -2739,31 +2854,31 @@
       <c r="D24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H24" s="31"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="34"/>
     </row>
     <row r="25" spans="1:10" ht="18">
       <c r="A25" s="2">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>56</v>
@@ -2771,28 +2886,28 @@
       <c r="F25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>114</v>
+      <c r="G25" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="18">
+    <row r="26" spans="1:10" ht="18.75" thickBot="1">
       <c r="A26" s="2">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>56</v>
@@ -2801,16 +2916,16 @@
         <v>56</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30">
+    <row r="27" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -2823,24 +2938,24 @@
       <c r="D27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>118</v>
+      <c r="E27" s="8" t="s">
+        <v>116</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="H27" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="I27" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="J27" s="27"/>
-    </row>
-    <row r="28" spans="1:10" ht="30">
+        <v>119</v>
+      </c>
+      <c r="H27" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="J27" s="34"/>
+    </row>
+    <row r="28" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -2853,20 +2968,20 @@
       <c r="D28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>119</v>
+      <c r="E28" s="8" t="s">
+        <v>117</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="H28" s="40"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="27"/>
-    </row>
-    <row r="29" spans="1:10" ht="30">
+        <v>120</v>
+      </c>
+      <c r="H28" s="42"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="34"/>
+    </row>
+    <row r="29" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -2879,20 +2994,20 @@
       <c r="D29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>120</v>
+      <c r="E29" s="8" t="s">
+        <v>118</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="H29" s="40"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="27"/>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" thickBot="1">
+        <v>121</v>
+      </c>
+      <c r="H29" s="42"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="34"/>
+    </row>
+    <row r="30" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -2905,21 +3020,21 @@
       <c r="D30" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="14" t="s">
-        <v>115</v>
+      <c r="E30" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H30" s="40"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="27"/>
+        <v>113</v>
+      </c>
+      <c r="H30" s="42"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="34"/>
     </row>
     <row r="31" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A31" s="2">
+      <c r="A31" s="14">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2931,27 +3046,25 @@
       <c r="D31" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>126</v>
+      <c r="E31" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G31" s="39" t="s">
+      <c r="G31" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="40" t="s">
-        <v>91</v>
-      </c>
-      <c r="I31" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="J31" s="30" t="s">
-        <v>129</v>
-      </c>
+      <c r="H31" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A32" s="2">
+      <c r="A32" s="14">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2963,21 +3076,25 @@
       <c r="D32" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E32" s="9" t="s">
-        <v>127</v>
+      <c r="E32" s="8" t="s">
+        <v>125</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="40"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="30"/>
+      <c r="H32" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="I32" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="J32" s="40"/>
     </row>
     <row r="33" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A33" s="2">
+      <c r="A33" s="14">
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2989,18 +3106,22 @@
       <c r="D33" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>128</v>
+      <c r="E33" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G33" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="H33" s="40"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="30"/>
+      <c r="H33" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="J33" s="40"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickTop="1">
       <c r="A34" s="2">
@@ -3015,20 +3136,20 @@
       <c r="D34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>133</v>
+      <c r="E34" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H34" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="I34" s="26" t="s">
-        <v>135</v>
+        <v>127</v>
+      </c>
+      <c r="H34" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="I34" s="32" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1">
@@ -3044,20 +3165,20 @@
       <c r="D35" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>132</v>
+      <c r="E35" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="H35" s="41"/>
-      <c r="I35" s="26"/>
+        <v>128</v>
+      </c>
+      <c r="H35" s="36"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A36" s="15">
+      <c r="A36" s="25">
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3067,7 +3188,7 @@
         <v>47</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>56</v>
@@ -3075,15 +3196,17 @@
       <c r="F36" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G36" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I36" s="2"/>
-      <c r="J36" s="22" t="s">
-        <v>202</v>
+      <c r="G36" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="18.75" thickTop="1">
@@ -3091,13 +3214,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>56</v>
@@ -3105,11 +3228,11 @@
       <c r="F37" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="13" t="s">
-        <v>114</v>
+      <c r="G37" s="12" t="s">
+        <v>112</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>56</v>
@@ -3120,13 +3243,13 @@
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>48</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>56</v>
@@ -3135,17 +3258,17 @@
         <v>56</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A39" s="15">
+      <c r="A39" s="25">
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -3155,7 +3278,7 @@
         <v>47</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>56</v>
@@ -3163,19 +3286,21 @@
       <c r="F39" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I39" s="2"/>
-      <c r="J39" s="22" t="s">
-        <v>202</v>
+      <c r="G39" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I39" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A40" s="15">
+      <c r="A40" s="14">
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -3185,29 +3310,27 @@
         <v>47</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="G40" s="16" t="s">
+      <c r="F40" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="G40" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I40" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>203</v>
-      </c>
+      <c r="H40" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="I40" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="J40" s="26"/>
     </row>
     <row r="41" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A41" s="15">
+      <c r="A41" s="25">
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -3216,26 +3339,30 @@
       <c r="C41" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="18" t="s">
-        <v>144</v>
+      <c r="D41" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F41" s="35" t="s">
-        <v>188</v>
-      </c>
-      <c r="G41" s="16" t="s">
+      <c r="F41" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="H41" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="18"/>
-    </row>
-    <row r="42" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
-      <c r="A42" s="15">
+      <c r="G41" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="I41" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="30.75" thickTop="1">
+      <c r="A42" s="14">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -3245,28 +3372,26 @@
         <v>47</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I42" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="J42" s="19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="F42" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="H42" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="I42" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="J42" s="26"/>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" s="2">
         <v>41</v>
       </c>
@@ -3280,25 +3405,23 @@
         <v>39</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F43" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G43" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="G43" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="J43" s="19" t="s">
+      <c r="H43" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="I43" s="25" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="J43" s="25"/>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="2">
         <v>42</v>
       </c>
@@ -3308,27 +3431,27 @@
       <c r="C44" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>150</v>
+      <c r="E44" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>144</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="H44" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="I44" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="J44" s="27"/>
-    </row>
-    <row r="45" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+        <v>146</v>
+      </c>
+      <c r="H44" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="I44" s="36" t="s">
+        <v>195</v>
+      </c>
+      <c r="J44" s="34"/>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="2">
         <v>43</v>
       </c>
@@ -3338,23 +3461,23 @@
       <c r="C45" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D45" s="42" t="s">
+      <c r="D45" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>149</v>
+      <c r="E45" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>143</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="H45" s="29"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="27"/>
-    </row>
-    <row r="46" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+        <v>147</v>
+      </c>
+      <c r="H45" s="43"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="34"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" thickBot="1">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -3376,18 +3499,16 @@
       <c r="G46" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H46" s="18" t="s">
-        <v>114</v>
+      <c r="H46" s="25" t="s">
+        <v>192</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J46" s="23" t="s">
-        <v>167</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A47" s="15">
+      <c r="A47" s="14">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -3399,27 +3520,27 @@
       <c r="D47" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E47" s="38" t="s">
-        <v>156</v>
+      <c r="E47" s="25" t="s">
+        <v>149</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="G47" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G47" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H47" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="I47" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="J47" s="30" t="s">
-        <v>172</v>
+      <c r="H47" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I47" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="J47" s="35" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A48" s="15">
+      <c r="A48" s="14">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -3431,18 +3552,20 @@
       <c r="D48" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="38" t="s">
-        <v>157</v>
+      <c r="E48" s="25" t="s">
+        <v>150</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="G48" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G48" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="H48" s="29"/>
-      <c r="I48" s="29"/>
-      <c r="J48" s="30"/>
+      <c r="H48" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
     </row>
     <row r="49" spans="1:10" ht="18.75" thickTop="1">
       <c r="A49" s="2">
@@ -3455,7 +3578,7 @@
         <v>48</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>56</v>
@@ -3464,10 +3587,10 @@
         <v>56</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>56</v>
@@ -3484,98 +3607,96 @@
         <v>48</v>
       </c>
       <c r="D50" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="I52" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="J52" s="16"/>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="I53" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="J53" s="16"/>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="22"/>
+      <c r="I54" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="J54" s="16"/>
+    </row>
+    <row r="55" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A55" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="I55" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="J55" s="16"/>
+    </row>
+    <row r="56" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A56" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="E50" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="I52" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="J52" s="18" t="s">
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="I56" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="J56" s="25" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
-      <c r="I53" s="44" t="s">
-        <v>195</v>
-      </c>
-      <c r="J53" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="43" t="s">
-        <v>168</v>
-      </c>
-      <c r="B54" s="43"/>
-      <c r="I54" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="J54" s="18" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="43" t="s">
-        <v>169</v>
-      </c>
-      <c r="B55" s="43"/>
-      <c r="C55" s="43"/>
-      <c r="D55" s="43"/>
-      <c r="I55" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="J55" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="36" t="s">
-        <v>170</v>
-      </c>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="I56" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="J56" s="18" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="I57" s="44" t="s">
-        <v>199</v>
+    <row r="57" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A57" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="I57" s="38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="I58" s="38" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="35">
+    <mergeCell ref="A55:E55"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A57:E57"/>
-    <mergeCell ref="H47:H48"/>
     <mergeCell ref="J47:J48"/>
     <mergeCell ref="I47:I48"/>
     <mergeCell ref="H34:H35"/>
@@ -3586,9 +3707,6 @@
     <mergeCell ref="H27:H30"/>
     <mergeCell ref="J27:J30"/>
     <mergeCell ref="I27:I30"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="I31:I33"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="I16:I19"/>
     <mergeCell ref="H16:H19"/>
@@ -3604,6 +3722,7 @@
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J7:J8"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Backup before updating supply symbols.
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
+++ b/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
@@ -2253,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G22" workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2985,7 +2985,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="18">
+    <row r="26" spans="1:10" ht="18.75" thickBot="1">
       <c r="A26" s="15">
         <v>24</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30">
+    <row r="27" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3033,7 +3033,7 @@
       <c r="F27" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="45" t="s">
         <v>119</v>
       </c>
       <c r="H27" s="37" t="s">
@@ -3044,8 +3044,8 @@
       </c>
       <c r="J27" s="34"/>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="2">
+    <row r="28" spans="1:10" ht="15.75" thickTop="1">
+      <c r="A28" s="15">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -3071,7 +3071,7 @@
       <c r="J28" s="34"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="2">
+      <c r="A29" s="15">
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -3097,7 +3097,7 @@
       <c r="J29" s="34"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A30" s="2">
+      <c r="A30" s="15">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -3594,7 +3594,7 @@
       <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="24">
+      <c r="A47" s="15">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -3624,7 +3624,7 @@
       <c r="J47" s="34"/>
     </row>
     <row r="48" spans="1:10">
-      <c r="A48" s="24">
+      <c r="A48" s="15">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">

</xml_diff>

<commit_message>
ADC pin assignment updated.
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
+++ b/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
@@ -1825,7 +1825,7 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1919,39 +1919,45 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2253,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2273,50 +2279,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="45"/>
+      <c r="G1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="45" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="9" t="s">
         <v>51</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:10" ht="30">
       <c r="A3" s="15">
@@ -2399,13 +2405,13 @@
       <c r="G5" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="J5" s="40" t="s">
+      <c r="J5" s="39" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2431,9 +2437,9 @@
       <c r="G6" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="40"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="15">
@@ -2457,13 +2463,13 @@
       <c r="G7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="38" t="s">
+      <c r="H7" s="41" t="s">
         <v>175</v>
       </c>
-      <c r="I7" s="38" t="s">
+      <c r="I7" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="J7" s="43" t="s">
+      <c r="J7" s="40" t="s">
         <v>177</v>
       </c>
     </row>
@@ -2489,9 +2495,9 @@
       <c r="G8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="43"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="15">
@@ -2553,7 +2559,7 @@
       <c r="I10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="44"/>
+      <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10" ht="18">
       <c r="A11" s="15">
@@ -2583,7 +2589,7 @@
       <c r="I11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="44"/>
+      <c r="J11" s="38"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="32.25" customHeight="1">
       <c r="A12" s="15">
@@ -2604,14 +2610,14 @@
       <c r="F12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>69</v>
+      <c r="G12" s="36" t="s">
+        <v>93</v>
       </c>
       <c r="H12" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>97</v>
+      <c r="I12" s="35" t="s">
+        <v>95</v>
       </c>
       <c r="J12" s="2"/>
     </row>
@@ -2634,14 +2640,14 @@
       <c r="F13" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>76</v>
+      <c r="G13" s="36" t="s">
+        <v>94</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>98</v>
+      <c r="I13" s="35" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30">
@@ -2663,14 +2669,14 @@
       <c r="F14" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>77</v>
+      <c r="G14" s="36" t="s">
+        <v>69</v>
       </c>
       <c r="H14" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>99</v>
+      <c r="I14" s="35" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30">
@@ -2692,14 +2698,14 @@
       <c r="F15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>78</v>
+      <c r="G15" s="36" t="s">
+        <v>77</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>100</v>
+      <c r="I15" s="35" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30">
@@ -2724,13 +2730,13 @@
       <c r="G16" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="H16" s="41" t="s">
+      <c r="H16" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="I16" s="38" t="s">
+      <c r="I16" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="44"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="15">
@@ -2754,9 +2760,9 @@
       <c r="G17" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="44"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="38"/>
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="A18" s="15">
@@ -2780,9 +2786,9 @@
       <c r="G18" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H18" s="41"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="44"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="38"/>
     </row>
     <row r="19" spans="1:10" ht="30">
       <c r="A19" s="15">
@@ -2806,9 +2812,9 @@
       <c r="G19" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="H19" s="41"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="44"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="38"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="15">
@@ -2829,14 +2835,14 @@
       <c r="F20" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>93</v>
+      <c r="G20" s="36" t="s">
+        <v>78</v>
       </c>
       <c r="H20" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>95</v>
+      <c r="I20" s="35" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2858,14 +2864,14 @@
       <c r="F21" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>94</v>
+      <c r="G21" s="36" t="s">
+        <v>76</v>
       </c>
       <c r="H21" s="24" t="s">
         <v>197</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>96</v>
+      <c r="I21" s="35" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="18">
@@ -2922,13 +2928,13 @@
       <c r="G23" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H23" s="42" t="s">
+      <c r="H23" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="I23" s="38" t="s">
+      <c r="I23" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="J23" s="44"/>
+      <c r="J23" s="38"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="15">
@@ -2952,9 +2958,9 @@
       <c r="G24" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="18">
       <c r="A25" s="15">
@@ -3036,13 +3042,13 @@
       <c r="G27" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="H27" s="38" t="s">
+      <c r="H27" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="I27" s="38" t="s">
+      <c r="I27" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="J27" s="44"/>
+      <c r="J27" s="38"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="15">
@@ -3066,9 +3072,9 @@
       <c r="G28" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="44"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="15">
@@ -3092,9 +3098,9 @@
       <c r="G29" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="44"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="41"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" thickBot="1">
       <c r="A30" s="15">
@@ -3118,9 +3124,9 @@
       <c r="G30" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="H30" s="39"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="44"/>
+      <c r="H30" s="48"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="31.5" thickTop="1" thickBot="1">
       <c r="A31" s="15">
@@ -3176,7 +3182,7 @@
       <c r="G32" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="35" t="s">
+      <c r="H32" s="46" t="s">
         <v>89</v>
       </c>
       <c r="I32" s="28" t="s">
@@ -3206,7 +3212,7 @@
       <c r="G33" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="H33" s="35"/>
+      <c r="H33" s="46"/>
       <c r="I33" s="24" t="s">
         <v>190</v>
       </c>
@@ -3233,10 +3239,10 @@
       <c r="G34" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H34" s="43" t="s">
+      <c r="H34" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="I34" s="38" t="s">
+      <c r="I34" s="41" t="s">
         <v>132</v>
       </c>
     </row>
@@ -3262,8 +3268,8 @@
       <c r="G35" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="H35" s="43"/>
-      <c r="I35" s="38"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="15">
@@ -3529,13 +3535,13 @@
       <c r="G44" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="H44" s="41" t="s">
+      <c r="H44" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="I44" s="45" t="s">
+      <c r="I44" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="J44" s="44"/>
+      <c r="J44" s="38"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="15">
@@ -3559,9 +3565,9 @@
       <c r="G45" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="H45" s="41"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="44"/>
+      <c r="H45" s="42"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="38"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="15">
@@ -3618,10 +3624,10 @@
       <c r="H47" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="I47" s="40" t="s">
+      <c r="I47" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="J47" s="44"/>
+      <c r="J47" s="38"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="15">
@@ -3648,8 +3654,8 @@
       <c r="H48" s="23" t="s">
         <v>171</v>
       </c>
-      <c r="I48" s="40"/>
-      <c r="J48" s="44"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="38"/>
     </row>
     <row r="49" spans="1:10" ht="18">
       <c r="A49" s="15">
@@ -3734,26 +3740,26 @@
       </c>
     </row>
     <row r="55" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A55" s="46" t="s">
+      <c r="A55" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="B55" s="46"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
       <c r="I55" s="15" t="s">
         <v>188</v>
       </c>
       <c r="J55" s="14"/>
     </row>
     <row r="56" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A56" s="46" t="s">
+      <c r="A56" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="B56" s="46"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="46"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
       <c r="I56" s="29" t="s">
         <v>173</v>
       </c>
@@ -3762,11 +3768,11 @@
       </c>
     </row>
     <row r="57" spans="1:10" ht="15.75" thickTop="1">
-      <c r="A57" s="44"/>
-      <c r="B57" s="44"/>
-      <c r="C57" s="44"/>
-      <c r="D57" s="44"/>
-      <c r="E57" s="44"/>
+      <c r="A57" s="38"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
       <c r="I57" s="26" t="s">
         <v>174</v>
       </c>
@@ -3781,16 +3787,23 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J7:J8"/>
     <mergeCell ref="J27:J30"/>
     <mergeCell ref="I27:I30"/>
     <mergeCell ref="J10:J11"/>
@@ -3800,23 +3813,16 @@
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="I23:I24"/>
     <mergeCell ref="J23:J24"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="H27:H30"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="I47:I48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Transistors drawn and checked.
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
+++ b/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="203">
   <si>
     <t>Pin #</t>
   </si>
@@ -1580,6 +1580,9 @@
   </si>
   <si>
     <t>Suspend (SUSP)</t>
+  </si>
+  <si>
+    <t>Wall present (ACPR)</t>
   </si>
 </sst>
 </file>
@@ -1678,7 +1681,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1703,12 +1706,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1776,7 +1773,7 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1874,48 +1871,45 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2216,8 +2210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2236,50 +2230,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="45"/>
-      <c r="G1" s="49" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="H1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="40" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="9" t="s">
         <v>51</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="49"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
     </row>
     <row r="3" spans="1:10" ht="30">
       <c r="A3" s="14">
@@ -2336,8 +2330,8 @@
       <c r="H4" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="I4" s="35" t="s">
-        <v>193</v>
+      <c r="I4" s="37" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -2362,13 +2356,13 @@
       <c r="G5" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="45" t="s">
         <v>160</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="43" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2394,9 +2388,9 @@
       <c r="G6" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="42"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="46"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="43"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14">
@@ -2426,7 +2420,7 @@
       <c r="I7" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="46" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2454,7 +2448,7 @@
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="41"/>
-      <c r="J8" s="40"/>
+      <c r="J8" s="46"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="14">
@@ -2516,7 +2510,7 @@
       <c r="I10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="39"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="11" spans="1:10" ht="18">
       <c r="A11" s="14">
@@ -2546,7 +2540,7 @@
       <c r="I11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="39"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="32.25" customHeight="1">
       <c r="A12" s="14">
@@ -2687,13 +2681,13 @@
       <c r="G16" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="44" t="s">
         <v>88</v>
       </c>
       <c r="I16" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="39"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="14">
@@ -2717,9 +2711,9 @@
       <c r="G17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H17" s="42"/>
+      <c r="H17" s="44"/>
       <c r="I17" s="41"/>
-      <c r="J17" s="39"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10" ht="30">
       <c r="A18" s="14">
@@ -2743,9 +2737,9 @@
       <c r="G18" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="42"/>
+      <c r="H18" s="44"/>
       <c r="I18" s="41"/>
-      <c r="J18" s="39"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" ht="30">
       <c r="A19" s="14">
@@ -2769,9 +2763,9 @@
       <c r="G19" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="H19" s="42"/>
+      <c r="H19" s="44"/>
       <c r="I19" s="41"/>
-      <c r="J19" s="39"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="14">
@@ -2885,13 +2879,13 @@
       <c r="G23" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="H23" s="44" t="s">
+      <c r="H23" s="48" t="s">
         <v>196</v>
       </c>
       <c r="I23" s="41" t="s">
         <v>106</v>
       </c>
-      <c r="J23" s="39"/>
+      <c r="J23" s="47"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="14">
@@ -2915,9 +2909,9 @@
       <c r="G24" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="H24" s="44"/>
+      <c r="H24" s="48"/>
       <c r="I24" s="41"/>
-      <c r="J24" s="39"/>
+      <c r="J24" s="47"/>
     </row>
     <row r="25" spans="1:10" ht="18">
       <c r="A25" s="14">
@@ -3005,7 +2999,7 @@
       <c r="I27" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="J27" s="39"/>
+      <c r="J27" s="47"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="14">
@@ -3031,7 +3025,7 @@
       </c>
       <c r="H28" s="41"/>
       <c r="I28" s="41"/>
-      <c r="J28" s="39"/>
+      <c r="J28" s="47"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="14">
@@ -3057,7 +3051,7 @@
       </c>
       <c r="H29" s="41"/>
       <c r="I29" s="41"/>
-      <c r="J29" s="39"/>
+      <c r="J29" s="47"/>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="14">
@@ -3081,9 +3075,9 @@
       <c r="G30" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H30" s="50"/>
+      <c r="H30" s="42"/>
       <c r="I30" s="41"/>
-      <c r="J30" s="39"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="14">
@@ -3137,7 +3131,7 @@
       <c r="G32" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="48" t="s">
+      <c r="H32" s="38" t="s">
         <v>88</v>
       </c>
       <c r="I32" s="26" t="s">
@@ -3167,7 +3161,7 @@
       <c r="G33" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H33" s="48"/>
+      <c r="H33" s="38"/>
       <c r="I33" s="22" t="s">
         <v>179</v>
       </c>
@@ -3194,7 +3188,7 @@
       <c r="G34" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="H34" s="40" t="s">
+      <c r="H34" s="46" t="s">
         <v>128</v>
       </c>
       <c r="I34" s="41" t="s">
@@ -3223,7 +3217,7 @@
       <c r="G35" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="H35" s="40"/>
+      <c r="H35" s="46"/>
       <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:10">
@@ -3333,7 +3327,7 @@
       <c r="F39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="37" t="s">
         <v>164</v>
       </c>
       <c r="H39" s="21" t="s">
@@ -3395,7 +3389,7 @@
       <c r="F41" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="G41" s="19" t="s">
+      <c r="G41" s="37" t="s">
         <v>165</v>
       </c>
       <c r="H41" s="21" t="s">
@@ -3457,7 +3451,7 @@
       <c r="F43" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="G43" s="19" t="s">
+      <c r="G43" s="37" t="s">
         <v>39</v>
       </c>
       <c r="H43" s="19" t="s">
@@ -3487,16 +3481,16 @@
       <c r="F44" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G44" s="5" t="s">
+      <c r="G44" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="H44" s="42" t="s">
+      <c r="H44" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="43" t="s">
+      <c r="I44" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="J44" s="39"/>
+      <c r="J44" s="47"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="14">
@@ -3520,9 +3514,9 @@
       <c r="G45" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="H45" s="42"/>
-      <c r="I45" s="43"/>
-      <c r="J45" s="39"/>
+      <c r="H45" s="44"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="47"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="14">
@@ -3540,16 +3534,16 @@
       <c r="E46" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F46" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G46" s="5" t="s">
+      <c r="F46" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="H46" s="19" t="s">
+      <c r="H46" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="I46" s="37" t="s">
         <v>145</v>
       </c>
       <c r="J46" s="20"/>
@@ -3570,19 +3564,19 @@
       <c r="E47" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="F47" s="5" t="s">
+      <c r="F47" s="37" t="s">
         <v>143</v>
       </c>
       <c r="G47" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="H47" s="51" t="s">
+      <c r="H47" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="I47" s="51" t="s">
+      <c r="I47" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="J47" s="39"/>
+      <c r="J47" s="47"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="14">
@@ -3600,19 +3594,19 @@
       <c r="E48" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="F48" s="5" t="s">
+      <c r="F48" s="37" t="s">
         <v>144</v>
       </c>
       <c r="G48" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="H48" s="51" t="s">
+      <c r="H48" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="I48" s="51" t="s">
-        <v>201</v>
-      </c>
-      <c r="J48" s="39"/>
+      <c r="I48" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="J48" s="47"/>
     </row>
     <row r="49" spans="1:10" ht="18">
       <c r="A49" s="14">
@@ -3630,16 +3624,16 @@
       <c r="E49" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F49" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G49" s="5" t="s">
+      <c r="F49" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="I49" s="2" t="s">
+      <c r="I49" s="37" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3695,43 +3689,69 @@
       <c r="J54" s="22"/>
     </row>
     <row r="55" spans="1:10">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="50" t="s">
         <v>153</v>
       </c>
-      <c r="B55" s="38"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
       <c r="I55" s="24" t="s">
         <v>166</v>
       </c>
       <c r="J55" s="13"/>
     </row>
     <row r="56" spans="1:10">
-      <c r="A56" s="38" t="s">
+      <c r="A56" s="50" t="s">
         <v>199</v>
       </c>
-      <c r="B56" s="38"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="38"/>
-      <c r="E56" s="38"/>
+      <c r="B56" s="50"/>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="50"/>
       <c r="I56" s="35" t="s">
         <v>175</v>
       </c>
       <c r="J56" s="19"/>
     </row>
     <row r="57" spans="1:10">
-      <c r="A57" s="39"/>
-      <c r="B57" s="39"/>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
+      <c r="A57" s="47"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
     </row>
     <row r="59" spans="1:10">
       <c r="B59" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J7:J8"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:F1"/>
@@ -3741,32 +3761,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="H27:H30"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A56:E56"/>
-    <mergeCell ref="A57:E57"/>
-    <mergeCell ref="J47:J48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Swapped PB4 with PB5 for I2C alert functionality.
</commit_message>
<xml_diff>
--- a/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
+++ b/hardware/PowerBoard/Document/STM32F10x Pin Assignment.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="343"/>
@@ -1634,8 +1634,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1727,7 +1727,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1752,12 +1752,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1930,15 +1924,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1948,33 +1967,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1985,6 +1979,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2063,6 +2062,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2097,6 +2097,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2272,14 +2273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:I19"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -2294,53 +2295,53 @@
     <col min="11" max="11" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="46"/>
-      <c r="G1" s="45" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
       <c r="E2" s="9" t="s">
         <v>51</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-    </row>
-    <row r="3" spans="1:10" ht="30">
+      <c r="G2" s="54"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="31">
         <v>1</v>
       </c>
@@ -2370,7 +2371,7 @@
       </c>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="31">
         <v>2</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="31">
         <v>3</v>
       </c>
@@ -2421,17 +2422,17 @@
       <c r="G5" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="50" t="s">
+      <c r="H5" s="46" t="s">
         <v>146</v>
       </c>
       <c r="I5" s="51" t="s">
         <v>151</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="J5" s="50" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="31">
         <v>4</v>
       </c>
@@ -2453,11 +2454,11 @@
       <c r="G6" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="50"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="51"/>
-      <c r="J6" s="49"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="J6" s="50"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="31">
         <v>5</v>
       </c>
@@ -2479,17 +2480,17 @@
       <c r="G7" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="H7" s="47" t="s">
+      <c r="H7" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="47" t="s">
+      <c r="I7" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="J7" s="52" t="s">
+      <c r="J7" s="44" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="31">
         <v>6</v>
       </c>
@@ -2511,11 +2512,11 @@
       <c r="G8" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="52"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="44"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="31">
         <v>7</v>
       </c>
@@ -2547,7 +2548,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18">
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" s="31">
         <v>8</v>
       </c>
@@ -2575,9 +2576,9 @@
       <c r="I10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="53"/>
-    </row>
-    <row r="11" spans="1:10" ht="18">
+      <c r="J10" s="43"/>
+    </row>
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>9</v>
       </c>
@@ -2605,9 +2606,9 @@
       <c r="I11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="53"/>
-    </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="32.25" customHeight="1">
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31">
         <v>10</v>
       </c>
@@ -2637,7 +2638,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" ht="30">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="31">
         <v>11</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30">
+    <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="31">
         <v>12</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="31">
         <v>13</v>
       </c>
@@ -2724,7 +2725,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="31">
         <v>14</v>
       </c>
@@ -2746,15 +2747,15 @@
       <c r="G16" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="H16" s="50" t="s">
+      <c r="H16" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="47" t="s">
+      <c r="I16" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="53"/>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="J16" s="43"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="31">
         <v>15</v>
       </c>
@@ -2776,11 +2777,11 @@
       <c r="G17" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="50"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="53"/>
-    </row>
-    <row r="18" spans="1:10" ht="30">
+      <c r="H17" s="46"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="43"/>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
         <v>16</v>
       </c>
@@ -2802,11 +2803,11 @@
       <c r="G18" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="50"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="53"/>
-    </row>
-    <row r="19" spans="1:10" ht="30">
+      <c r="H18" s="46"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="43"/>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="31">
         <v>17</v>
       </c>
@@ -2828,11 +2829,11 @@
       <c r="G19" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="50"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="53"/>
-    </row>
-    <row r="20" spans="1:10" ht="30">
+      <c r="H19" s="46"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="43"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="31">
         <v>18</v>
       </c>
@@ -2861,7 +2862,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="31">
         <v>19</v>
       </c>
@@ -2890,7 +2891,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="18">
+    <row r="22" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="31">
         <v>20</v>
       </c>
@@ -2922,7 +2923,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="31">
         <v>21</v>
       </c>
@@ -2944,15 +2945,15 @@
       <c r="G23" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="H23" s="54" t="s">
+      <c r="H23" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="I23" s="47" t="s">
+      <c r="I23" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="J23" s="53"/>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="J23" s="43"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="31">
         <v>22</v>
       </c>
@@ -2974,11 +2975,11 @@
       <c r="G24" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H24" s="54"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="53"/>
-    </row>
-    <row r="25" spans="1:10" ht="18">
+      <c r="H24" s="48"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="43"/>
+    </row>
+    <row r="25" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" s="31">
         <v>23</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="18">
+    <row r="26" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" s="31">
         <v>24</v>
       </c>
@@ -3036,7 +3037,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30">
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="31">
         <v>25</v>
       </c>
@@ -3058,15 +3059,15 @@
       <c r="G27" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="H27" s="47" t="s">
+      <c r="H27" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="I27" s="47" t="s">
+      <c r="I27" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="J27" s="53"/>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="J27" s="43"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="31">
         <v>26</v>
       </c>
@@ -3088,11 +3089,11 @@
       <c r="G28" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="H28" s="47"/>
-      <c r="I28" s="47"/>
-      <c r="J28" s="53"/>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="43"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="31">
         <v>27</v>
       </c>
@@ -3114,11 +3115,11 @@
       <c r="G29" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="H29" s="47"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="53"/>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="43"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="31">
         <v>28</v>
       </c>
@@ -3140,11 +3141,11 @@
       <c r="G30" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="H30" s="48"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="53"/>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="H30" s="55"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="43"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="31">
         <v>29</v>
       </c>
@@ -3174,7 +3175,7 @@
       </c>
       <c r="J31" s="29"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="31">
         <v>30</v>
       </c>
@@ -3196,15 +3197,15 @@
       <c r="G32" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H32" s="44" t="s">
+      <c r="H32" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="I32" s="43" t="s">
+      <c r="I32" s="52" t="s">
         <v>193</v>
       </c>
       <c r="J32" s="23"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="31">
         <v>31</v>
       </c>
@@ -3226,11 +3227,11 @@
       <c r="G33" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H33" s="44"/>
-      <c r="I33" s="43"/>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="40">
+      <c r="H33" s="53"/>
+      <c r="I33" s="52"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="31">
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -3251,15 +3252,15 @@
       <c r="G34" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="H34" s="52" t="s">
+      <c r="H34" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="I34" s="47" t="s">
+      <c r="I34" s="45" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="40">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -3280,10 +3281,10 @@
       <c r="G35" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="H35" s="52"/>
-      <c r="I35" s="47"/>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="H35" s="44"/>
+      <c r="I35" s="45"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="31">
         <v>34</v>
       </c>
@@ -3313,7 +3314,7 @@
       </c>
       <c r="J36" s="18"/>
     </row>
-    <row r="37" spans="1:10" ht="18">
+    <row r="37" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="31">
         <v>35</v>
       </c>
@@ -3342,7 +3343,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="18">
+    <row r="38" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="31">
         <v>36</v>
       </c>
@@ -3371,7 +3372,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="31">
         <v>37</v>
       </c>
@@ -3401,7 +3402,7 @@
       </c>
       <c r="J39" s="18"/>
     </row>
-    <row r="40" spans="1:10" ht="30">
+    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="31">
         <v>38</v>
       </c>
@@ -3433,7 +3434,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="30">
+    <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="31">
         <v>39</v>
       </c>
@@ -3463,7 +3464,7 @@
       </c>
       <c r="J41" s="18"/>
     </row>
-    <row r="42" spans="1:10" ht="30">
+    <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="31">
         <v>40</v>
       </c>
@@ -3485,17 +3486,14 @@
       <c r="G42" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="H42" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="J42" s="21" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="H42" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="I42" s="42" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="31">
         <v>41</v>
       </c>
@@ -3517,15 +3515,17 @@
       <c r="G43" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="H43" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="I43" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="J43" s="18"/>
-    </row>
-    <row r="44" spans="1:10" ht="15" customHeight="1">
+      <c r="H43" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="I43" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="J43" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="31">
         <v>42</v>
       </c>
@@ -3547,15 +3547,15 @@
       <c r="G44" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="H44" s="50" t="s">
+      <c r="H44" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="I44" s="55" t="s">
+      <c r="I44" s="47" t="s">
         <v>172</v>
       </c>
-      <c r="J44" s="53"/>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="J44" s="43"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="31">
         <v>43</v>
       </c>
@@ -3577,11 +3577,11 @@
       <c r="G45" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="H45" s="50"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="53"/>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="H45" s="46"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="43"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="31">
         <v>44</v>
       </c>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="J46" s="19"/>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1">
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31">
         <v>45</v>
       </c>
@@ -3639,9 +3639,9 @@
       <c r="I47" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="J47" s="53"/>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="J47" s="43"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="31">
         <v>46</v>
       </c>
@@ -3669,9 +3669,9 @@
       <c r="I48" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="J48" s="53"/>
-    </row>
-    <row r="49" spans="1:10" ht="18">
+      <c r="J48" s="43"/>
+    </row>
+    <row r="49" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" s="31">
         <v>47</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="18">
+    <row r="50" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="A50" s="31">
         <v>48</v>
       </c>
@@ -3729,19 +3729,23 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I52" s="31" t="s">
         <v>184</v>
       </c>
       <c r="J52" s="13"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I53" s="31" t="s">
         <v>185</v>
       </c>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="35"/>
       <c r="B54" s="35"/>
       <c r="C54" s="35"/>
@@ -3752,18 +3756,18 @@
       </c>
       <c r="J54" s="21"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
-      <c r="I55" s="41" t="s">
+      <c r="I55" s="40" t="s">
         <v>157</v>
       </c>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -3774,53 +3778,31 @@
       </c>
       <c r="J56" s="18"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
-      <c r="I57" s="42" t="s">
+      <c r="I57" s="41" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="35"/>
       <c r="B58" s="35"/>
       <c r="C58" s="35"/>
       <c r="D58" s="35"/>
       <c r="E58" s="35"/>
-      <c r="I58" s="42" t="s">
+      <c r="I58" s="41" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B59" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="J47:J48"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="H44:H45"/>
-    <mergeCell ref="I44:I45"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="J27:J30"/>
-    <mergeCell ref="I27:I30"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J7:J8"/>
     <mergeCell ref="I32:I33"/>
     <mergeCell ref="H32:H33"/>
     <mergeCell ref="G1:G2"/>
@@ -3832,6 +3814,28 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="H27:H30"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J27:J30"/>
+    <mergeCell ref="I27:I30"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="J47:J48"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="H44:H45"/>
+    <mergeCell ref="I44:I45"/>
+    <mergeCell ref="J44:J45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3839,24 +3843,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>